<commit_message>
SoGo NS readings are done
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_Performance.xlsx
+++ b/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_Performance.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A85F46F-6A60-4087-832B-E44EB17B9D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A626F5D-37EF-439C-9246-BF8D9DADEE38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Users" sheetId="2" r:id="rId3"/>
     <sheet name="PerformanceTC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="121">
   <si>
     <t>Environment</t>
   </si>
@@ -91,12 +91,6 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>Expected2</t>
-  </si>
-  <si>
-    <t>Expected3</t>
-  </si>
-  <si>
     <t>https://www.sogosurvey.com/</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>Static Home</t>
   </si>
   <si>
-    <t>Access https://www.sogosurvey.com/</t>
-  </si>
-  <si>
     <t>Note page load time</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>Click Login Button</t>
   </si>
   <si>
-    <t>refer image https://zarcacom-my.sharepoint.com/:i:/g/personal/abhandi_zarca_com/EboZrPEb3zdFob6SA6dnJ4MBE90mWHtLq5h_3ng86ngtcA</t>
-  </si>
-  <si>
     <t>SoGo@NS3196</t>
   </si>
   <si>
@@ -145,10 +133,6 @@
     <t>Platform Log in</t>
   </si>
   <si>
-    <t xml:space="preserve">Access https://www.sogosurvey.com/static/nogin.aspx
-Enter Credentials and Login to platform  </t>
-  </si>
-  <si>
     <t>Note the Load time of Login</t>
   </si>
   <si>
@@ -158,10 +142,6 @@
     <t>Top Differentiating Features</t>
   </si>
   <si>
-    <t xml:space="preserve">refer image https://zarcacom-my.sharepoint.com/:i:/g/personal/abhandi_zarca_com/EU3aSvD27i5OhaaMi1RTbaUBsw9l_UGXziyxk8rlvNHdfA?e=OUGRn3
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Note page load time </t>
   </si>
   <si>
@@ -171,58 +151,241 @@
     <t>Pricing - Free&amp;Paid Plans</t>
   </si>
   <si>
-    <t>refer image https://zarcacom-my.sharepoint.com/:i:/g/personal/abhandi_zarca_com/EQ7-q0jBKZlHnUb2MLNs6DABDlEKbTnci8Q2Q8tDzbOp-w</t>
-  </si>
-  <si>
     <t>Performance_TC6</t>
   </si>
   <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Performance_TC7</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>Gaurav,Golatkar,test_username,GVG3196@test,testemail@gmail.com</t>
+  </si>
+  <si>
+    <t>Performance_TC8</t>
+  </si>
+  <si>
+    <t>Load SM Tab</t>
+  </si>
+  <si>
+    <t>Night support readings,2759</t>
+  </si>
+  <si>
+    <t>Performance_TC9</t>
+  </si>
+  <si>
+    <t>Depositing a Question in QB</t>
+  </si>
+  <si>
+    <t>Performance_TC10</t>
+  </si>
+  <si>
+    <t>Night support readings,2759,Additional suggestions do you have for improving the support for new teachers at this school</t>
+  </si>
+  <si>
+    <t>Performance_TC11</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Add Comment</t>
+  </si>
+  <si>
+    <t>Delete Comment</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Performance_TC12</t>
+  </si>
+  <si>
+    <t>Move Page</t>
+  </si>
+  <si>
+    <t>Night support readings,2759,1</t>
+  </si>
+  <si>
+    <t>Performance_TC13</t>
+  </si>
+  <si>
+    <t>Move Matrix Grid</t>
+  </si>
+  <si>
+    <t>Performance_TC14</t>
+  </si>
+  <si>
+    <t>Load DM Tab</t>
+  </si>
+  <si>
+    <t>Performance_TC15</t>
+  </si>
+  <si>
+    <t>Load RM tab</t>
+  </si>
+  <si>
+    <t>Cutomer Feedback,2721</t>
+  </si>
+  <si>
+    <t>Performance_TC16</t>
+  </si>
+  <si>
+    <t>Load OMNI Report</t>
+  </si>
+  <si>
+    <t>Performance_TC17</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Capture page load time of Static Home Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Login Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Top Differentiating Feature Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Pricing Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Registration Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Billing Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Home Page (Platform login)</t>
+  </si>
+  <si>
+    <t>Capture the page load time of SM Tab</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Depositing in Question Bank</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Add Comment</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Delete Comment</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Move Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of moving Matrix Grid question</t>
+  </si>
+  <si>
+    <t>Capture the page load time of DM Tab</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Report Tab</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Omni Report</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Logout</t>
+  </si>
+  <si>
+    <t>Reading 1</t>
+  </si>
+  <si>
+    <t>Reading 2</t>
+  </si>
+  <si>
+    <t>Reading 3</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>12.04</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>5.05</t>
+  </si>
+  <si>
+    <t>4.87</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7.77</t>
+  </si>
+  <si>
+    <t>2.98</t>
+  </si>
+  <si>
+    <t>3.74</t>
+  </si>
+  <si>
+    <t>2.93</t>
+  </si>
+  <si>
+    <t>12.55</t>
+  </si>
+  <si>
+    <t>6.65</t>
+  </si>
+  <si>
+    <t>2.42</t>
+  </si>
+  <si>
+    <t>16.27</t>
+  </si>
+  <si>
+    <t>7.9</t>
+  </si>
+  <si>
+    <t>4.06</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Registration</t>
-  </si>
-  <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>TestData</t>
-  </si>
-  <si>
-    <t>Performance_TC7</t>
-  </si>
-  <si>
-    <t>Billing</t>
-  </si>
-  <si>
-    <t>Gaurav,Golatkar,test_username,GVG3196@test,testemail@gmail.com</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>10.02</t>
-  </si>
-  <si>
-    <t>6.03</t>
-  </si>
-  <si>
-    <t>25.43</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Billing - Address field not present on page.</t>
-  </si>
-  <si>
-    <t>5.35</t>
-  </si>
-  <si>
-    <t>6.71</t>
+    <t>3.88</t>
+  </si>
+  <si>
+    <t>3.32</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>2.83</t>
+  </si>
+  <si>
+    <t>2.96</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>3.05</t>
+  </si>
+  <si>
+    <t>2.51</t>
   </si>
 </sst>
 </file>
@@ -230,7 +393,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,30 +487,8 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="42">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,67 +513,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -610,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -620,6 +701,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
@@ -638,14 +720,6 @@
     <xf numFmtId="0" fontId="14" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -956,7 +1030,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1045,10 +1119,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -1063,10 +1137,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1157,11 @@
     <col min="10" max="10" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="13.5703125" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="13" max="15" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="13" max="16" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="111.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1178,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>16</v>
@@ -1118,30 +1193,33 @@
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1153,35 +1231,45 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>52</v>
+        <v>25</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L2" s="8"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M2" s="4">
+        <v>4.78</v>
+      </c>
+      <c r="N2" s="1">
+        <v>4.28</v>
+      </c>
+      <c r="O2" s="4">
+        <v>3.72</v>
+      </c>
+      <c r="P2" s="9">
+        <f>AVERAGE(M2:O2)</f>
+        <v>4.2600000000000007</v>
+      </c>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -1193,35 +1281,45 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="4">
+        <v>3.18</v>
+      </c>
+      <c r="N3" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="P3" s="9">
+        <f t="shared" ref="P3:P18" si="0">AVERAGE(M3:O3)</f>
+        <v>2.1933333333333334</v>
+      </c>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1233,35 +1331,45 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L4" s="8"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M4" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>8.98</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" si="0"/>
+        <v>9.1266666666666669</v>
+      </c>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -1273,35 +1381,45 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L5" s="8"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M5" s="4">
+        <v>6.32</v>
+      </c>
+      <c r="N5" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="O5" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="P5" s="9">
+        <f t="shared" si="0"/>
+        <v>4.7766666666666664</v>
+      </c>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -1313,116 +1431,682 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>52</v>
+        <v>25</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L6" s="8"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M6" s="4">
+        <v>3.01</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="O6" s="4">
+        <v>3.82</v>
+      </c>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7766666666666668</v>
+      </c>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="33" t="s">
-        <v>52</v>
+        <v>25</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L7" s="8"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M7" s="4">
+        <v>4.63</v>
+      </c>
+      <c r="N7" s="1">
+        <v>5.03</v>
+      </c>
+      <c r="O7" s="4">
+        <v>3.97</v>
+      </c>
+      <c r="P7" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5433333333333339</v>
+      </c>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="4">
+        <v>3.44</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5.65</v>
+      </c>
+      <c r="O8" s="4">
+        <v>4.75</v>
+      </c>
+      <c r="P8" s="9">
+        <f t="shared" si="0"/>
+        <v>4.6133333333333333</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="4">
+        <v>9.69</v>
+      </c>
+      <c r="N9" s="1">
+        <v>9.52</v>
+      </c>
+      <c r="O9" s="4">
+        <v>7.71</v>
+      </c>
+      <c r="P9" s="9">
+        <f t="shared" si="0"/>
+        <v>8.9733333333333345</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="8"/>
+      <c r="M10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2866666666666668</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="31" t="s">
+      <c r="K11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="4">
+        <v>4.01</v>
+      </c>
+      <c r="N11" s="1">
+        <v>2.77</v>
+      </c>
+      <c r="O11" s="4">
+        <v>2.98</v>
+      </c>
+      <c r="P11" s="9">
+        <f t="shared" si="0"/>
+        <v>3.2533333333333334</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="H12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="4">
+        <v>3.85</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2.57</v>
+      </c>
+      <c r="O12" s="4">
+        <v>2.94</v>
+      </c>
+      <c r="P12" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1199999999999997</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="4">
+        <v>3.68</v>
+      </c>
+      <c r="N13" s="1">
+        <v>3.22</v>
+      </c>
+      <c r="O13" s="4">
+        <v>3.94</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6133333333333333</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="4">
+        <v>5.58</v>
+      </c>
+      <c r="N14" s="1">
+        <v>3.56</v>
+      </c>
+      <c r="O14" s="4">
+        <v>3.98</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" si="0"/>
+        <v>4.373333333333334</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="B15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>4.51</v>
+      </c>
+      <c r="O15" s="4">
+        <v>4.05</v>
+      </c>
+      <c r="P15" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5866666666666669</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L16" s="8"/>
+      <c r="M16" s="4">
+        <v>7.06</v>
+      </c>
+      <c r="N16" s="1">
+        <v>5.94</v>
+      </c>
+      <c r="O16" s="4">
+        <v>4.41</v>
+      </c>
+      <c r="P16" s="9">
+        <f t="shared" si="0"/>
+        <v>5.8033333333333337</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="4">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1.81</v>
+      </c>
+      <c r="P17" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0133333333333336</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="4">
+        <v>1.34</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1.96</v>
+      </c>
+      <c r="O18" s="4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="P18" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4866666666666666</v>
+      </c>
+      <c r="Q18" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{3A059418-576A-4680-B69E-251A95BCE337}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{3BA5E488-EB21-4F2D-B962-8635BBD138AA}"/>
+    <hyperlink ref="H5" r:id="rId3" display="Capture the page load time of Top Differentiating Feature Page" xr:uid="{62ADDCF6-848E-4237-AE58-9E5BF45C8E08}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{278DACE7-0617-4E51-BA65-0F48F54F1E8D}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{514B384F-5A6A-4387-AAD6-888C94EAFB5C}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{1C1F578E-8AF9-4650-B0AA-4E3A40B2CCB0}"/>
+    <hyperlink ref="H4" r:id="rId7" xr:uid="{BC85C1A0-DC3F-411A-B7E7-A962A7B78906}"/>
+    <hyperlink ref="H9:H17" r:id="rId8" display="Capture the page load time of Billing Page" xr:uid="{54DBFD5C-3893-46EB-B168-219D8D340230}"/>
+    <hyperlink ref="H18" r:id="rId9" xr:uid="{52C200CA-3D6B-4C68-B2D7-720B7B62D7E5}"/>
+    <hyperlink ref="H9" r:id="rId10" xr:uid="{12F64291-2B44-4FE9-9FC5-F15E0A6179BB}"/>
+    <hyperlink ref="H10" r:id="rId11" xr:uid="{C3CDB8C7-22F6-4A93-8489-39804E6E5089}"/>
+    <hyperlink ref="H11" r:id="rId12" xr:uid="{3A307E56-912E-4BD7-84F6-142F5CE70D44}"/>
+    <hyperlink ref="H12" r:id="rId13" xr:uid="{3CF3D5C6-EE29-4CA5-A140-5345B546BBF2}"/>
+    <hyperlink ref="H13" r:id="rId14" xr:uid="{D3A19956-AD04-4722-A899-93773A88010B}"/>
+    <hyperlink ref="H14" r:id="rId15" xr:uid="{85BE0BC5-8601-470F-AB7B-872DC1889239}"/>
+    <hyperlink ref="H15" r:id="rId16" xr:uid="{E1C4BCDC-809D-4A28-8C0F-4A60F2FE1AC4}"/>
+    <hyperlink ref="H16" r:id="rId17" xr:uid="{7A02DCFF-3EA9-410D-8739-85D21E7A2E3A}"/>
+    <hyperlink ref="H17" r:id="rId18" xr:uid="{CBAF6A21-DBA0-4470-A06D-8260B468E5BE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>